<commit_message>
seperately back up the paper draft latex until before incorporating SV and structural estimations. Then started working on InfVar.tex with new abstract.
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/UCSVestM.xlsx
+++ b/workingfolder/OtherData/UCSVestM.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -38,14 +38,30 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>